<commit_message>
Added manager run sort. 增加管理者运行排序
</commit_message>
<xml_diff>
--- a/Tools/LubanTools/DataTables/Lc_Datas/Lc.xlsx
+++ b/Tools/LubanTools/DataTables/Lc_Datas/Lc.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="674" uniqueCount="371">
   <si>
     <t>##var</t>
   </si>
@@ -241,6 +241,12 @@
   </si>
   <si>
     <t>颜色</t>
+  </si>
+  <si>
+    <t>Close</t>
+  </si>
+  <si>
+    <t>关闭</t>
   </si>
   <si>
     <t>Count</t>
@@ -2128,12 +2134,12 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Y172"/>
+  <dimension ref="A1:Y173"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A124" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="5" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="E132" sqref="E132"/>
+      <selection pane="bottomLeft" activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -2773,18 +2779,18 @@
         <v>84</v>
       </c>
       <c r="E38" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="39" spans="2:5">
       <c r="B39" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" t="s">
         <v>87</v>
       </c>
-      <c r="C39" t="s">
-        <v>88</v>
-      </c>
       <c r="D39" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E39" t="s">
         <v>88</v>
@@ -2927,18 +2933,18 @@
         <v>107</v>
       </c>
       <c r="E49" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" t="s">
+        <v>109</v>
+      </c>
+      <c r="C50" t="s">
         <v>110</v>
       </c>
-      <c r="C50" t="s">
-        <v>111</v>
-      </c>
       <c r="D50" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E50" t="s">
         <v>111</v>
@@ -2963,27 +2969,27 @@
         <v>114</v>
       </c>
       <c r="C52" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
       <c r="D52" t="s">
         <v>114</v>
       </c>
       <c r="E52" t="s">
-        <v>11</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="2:5">
       <c r="B53" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="C53" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53" t="s">
         <v>116</v>
       </c>
-      <c r="D53" t="s">
-        <v>115</v>
-      </c>
       <c r="E53" t="s">
-        <v>116</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="2:5">
@@ -3064,7 +3070,7 @@
         <v>128</v>
       </c>
       <c r="D59" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="E59" t="s">
         <v>128</v>
@@ -3072,16 +3078,16 @@
     </row>
     <row r="60" spans="2:5">
       <c r="B60" t="s">
+        <v>129</v>
+      </c>
+      <c r="C60" t="s">
         <v>130</v>
       </c>
-      <c r="C60" t="s">
+      <c r="D60" t="s">
         <v>131</v>
       </c>
-      <c r="D60" t="s">
+      <c r="E60" t="s">
         <v>130</v>
-      </c>
-      <c r="E60" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="61" spans="2:5">
@@ -3165,18 +3171,18 @@
         <v>142</v>
       </c>
       <c r="E66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="67" spans="2:5">
       <c r="B67" t="s">
+        <v>144</v>
+      </c>
+      <c r="C67" t="s">
         <v>145</v>
       </c>
-      <c r="C67" t="s">
-        <v>146</v>
-      </c>
       <c r="D67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E67" t="s">
         <v>146</v>
@@ -3221,18 +3227,18 @@
         <v>151</v>
       </c>
       <c r="E70" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="71" spans="2:5">
       <c r="B71" t="s">
+        <v>153</v>
+      </c>
+      <c r="C71" t="s">
         <v>154</v>
       </c>
-      <c r="C71" t="s">
-        <v>155</v>
-      </c>
       <c r="D71" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="E71" t="s">
         <v>155</v>
@@ -3249,18 +3255,18 @@
         <v>156</v>
       </c>
       <c r="E72" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="73" spans="2:5">
       <c r="B73" t="s">
+        <v>158</v>
+      </c>
+      <c r="C73" t="s">
         <v>159</v>
       </c>
-      <c r="C73" t="s">
-        <v>160</v>
-      </c>
       <c r="D73" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="E73" t="s">
         <v>160</v>
@@ -3274,18 +3280,18 @@
         <v>162</v>
       </c>
       <c r="D74" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E74" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="75" spans="2:5">
       <c r="B75" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C75" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="D75" t="s">
         <v>165</v>
@@ -3403,18 +3409,18 @@
         <v>181</v>
       </c>
       <c r="E83" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="84" spans="2:5">
       <c r="B84" t="s">
+        <v>183</v>
+      </c>
+      <c r="C84" t="s">
         <v>184</v>
       </c>
-      <c r="C84" t="s">
-        <v>185</v>
-      </c>
       <c r="D84" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="E84" t="s">
         <v>185</v>
@@ -3495,38 +3501,38 @@
         <v>196</v>
       </c>
       <c r="C90" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
       <c r="D90" t="s">
         <v>196</v>
       </c>
       <c r="E90" t="s">
-        <v>33</v>
+        <v>197</v>
       </c>
     </row>
     <row r="91" spans="2:5">
       <c r="B91" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C91" t="s">
+        <v>33</v>
+      </c>
+      <c r="D91" t="s">
         <v>198</v>
       </c>
-      <c r="D91" t="s">
-        <v>197</v>
-      </c>
       <c r="E91" t="s">
-        <v>199</v>
+        <v>33</v>
       </c>
     </row>
     <row r="92" spans="2:5">
       <c r="B92" t="s">
+        <v>199</v>
+      </c>
+      <c r="C92" t="s">
         <v>200</v>
       </c>
-      <c r="C92" t="s">
-        <v>201</v>
-      </c>
       <c r="D92" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E92" t="s">
         <v>201</v>
@@ -3652,7 +3658,7 @@
         <v>219</v>
       </c>
       <c r="D101" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="E101" t="s">
         <v>219</v>
@@ -3660,24 +3666,24 @@
     </row>
     <row r="102" spans="2:5">
       <c r="B102" t="s">
+        <v>220</v>
+      </c>
+      <c r="C102" t="s">
         <v>221</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>222</v>
       </c>
-      <c r="D102" t="s">
-        <v>223</v>
-      </c>
       <c r="E102" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="103" spans="2:5">
       <c r="B103" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C103" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="D103" t="s">
         <v>225</v>
@@ -3697,18 +3703,18 @@
         <v>227</v>
       </c>
       <c r="E104" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="105" spans="2:5">
       <c r="B105" t="s">
+        <v>229</v>
+      </c>
+      <c r="C105" t="s">
         <v>230</v>
       </c>
-      <c r="C105" t="s">
-        <v>231</v>
-      </c>
       <c r="D105" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="E105" t="s">
         <v>231</v>
@@ -3893,18 +3899,18 @@
         <v>256</v>
       </c>
       <c r="E118" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="2:5">
       <c r="B119" t="s">
+        <v>258</v>
+      </c>
+      <c r="C119" t="s">
         <v>259</v>
       </c>
-      <c r="C119" t="s">
-        <v>260</v>
-      </c>
       <c r="D119" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E119" t="s">
         <v>260</v>
@@ -4005,7 +4011,7 @@
         <v>273</v>
       </c>
       <c r="E126" t="s">
-        <v>98</v>
+        <v>274</v>
       </c>
     </row>
     <row r="127" spans="2:5">
@@ -4013,27 +4019,27 @@
         <v>275</v>
       </c>
       <c r="C127" t="s">
-        <v>28</v>
+        <v>276</v>
       </c>
       <c r="D127" t="s">
         <v>275</v>
       </c>
       <c r="E127" t="s">
-        <v>28</v>
+        <v>100</v>
       </c>
     </row>
     <row r="128" spans="2:5">
       <c r="B128" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="C128" t="s">
+        <v>28</v>
+      </c>
+      <c r="D128" t="s">
         <v>277</v>
       </c>
-      <c r="D128" t="s">
-        <v>276</v>
-      </c>
       <c r="E128" t="s">
-        <v>277</v>
+        <v>28</v>
       </c>
     </row>
     <row r="129" spans="2:5">
@@ -4229,18 +4235,18 @@
         <v>304</v>
       </c>
       <c r="E142" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="143" spans="2:5">
       <c r="B143" t="s">
+        <v>306</v>
+      </c>
+      <c r="C143" t="s">
         <v>307</v>
       </c>
-      <c r="C143" t="s">
-        <v>308</v>
-      </c>
       <c r="D143" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="E143" t="s">
         <v>308</v>
@@ -4313,18 +4319,18 @@
         <v>317</v>
       </c>
       <c r="E148" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="149" spans="2:5">
       <c r="B149" t="s">
+        <v>319</v>
+      </c>
+      <c r="C149" t="s">
         <v>320</v>
       </c>
-      <c r="C149" t="s">
-        <v>321</v>
-      </c>
       <c r="D149" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="E149" t="s">
         <v>321</v>
@@ -4484,136 +4490,150 @@
         <v>343</v>
       </c>
     </row>
-    <row r="161" s="3" customFormat="1" spans="1:1">
-      <c r="A161" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="162" s="3" customFormat="1" spans="1:5">
+    <row r="161" spans="2:5">
+      <c r="B161" t="s">
+        <v>344</v>
+      </c>
+      <c r="C161" t="s">
+        <v>345</v>
+      </c>
+      <c r="D161" t="s">
+        <v>344</v>
+      </c>
+      <c r="E161" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="162" s="3" customFormat="1" spans="1:1">
       <c r="A162" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B162" s="10" t="s">
-        <v>344</v>
-      </c>
-      <c r="C162" s="10"/>
-      <c r="D162" s="10"/>
-      <c r="E162" s="10"/>
-    </row>
-    <row r="163" spans="2:5">
-      <c r="B163" t="s">
-        <v>345</v>
-      </c>
-      <c r="C163" t="s">
+    </row>
+    <row r="163" s="3" customFormat="1" spans="1:5">
+      <c r="A163" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B163" s="10" t="s">
         <v>346</v>
       </c>
-      <c r="D163" t="s">
-        <v>347</v>
-      </c>
-      <c r="E163" t="s">
-        <v>346</v>
-      </c>
+      <c r="C163" s="10"/>
+      <c r="D163" s="10"/>
+      <c r="E163" s="10"/>
     </row>
     <row r="164" spans="2:5">
       <c r="B164" t="s">
+        <v>347</v>
+      </c>
+      <c r="C164" t="s">
         <v>348</v>
       </c>
-      <c r="C164" t="s">
+      <c r="D164" t="s">
         <v>349</v>
       </c>
-      <c r="D164" t="s">
+      <c r="E164" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="165" spans="2:5">
+      <c r="B165" t="s">
         <v>350</v>
       </c>
-      <c r="E164" t="s">
+      <c r="C165" t="s">
         <v>351</v>
       </c>
-    </row>
-    <row r="165" s="3" customFormat="1" spans="1:1">
-      <c r="A165" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="166" s="3" customFormat="1" spans="1:5">
+      <c r="D165" t="s">
+        <v>352</v>
+      </c>
+      <c r="E165" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="166" s="3" customFormat="1" spans="1:1">
       <c r="A166" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B166" s="10" t="s">
-        <v>352</v>
-      </c>
-      <c r="C166" s="10"/>
-      <c r="D166" s="10"/>
-      <c r="E166" s="10"/>
-    </row>
-    <row r="167" spans="2:5">
-      <c r="B167" t="s">
-        <v>353</v>
-      </c>
-      <c r="C167" t="s">
+    </row>
+    <row r="167" s="3" customFormat="1" spans="1:5">
+      <c r="A167" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B167" s="10" t="s">
         <v>354</v>
       </c>
-      <c r="D167" t="s">
-        <v>355</v>
-      </c>
-      <c r="E167" t="s">
-        <v>356</v>
-      </c>
+      <c r="C167" s="10"/>
+      <c r="D167" s="10"/>
+      <c r="E167" s="10"/>
     </row>
     <row r="168" spans="2:5">
       <c r="B168" t="s">
+        <v>355</v>
+      </c>
+      <c r="C168" t="s">
+        <v>356</v>
+      </c>
+      <c r="D168" t="s">
         <v>357</v>
       </c>
-      <c r="C168" t="s">
+      <c r="E168" t="s">
         <v>358</v>
-      </c>
-      <c r="D168" t="s">
-        <v>359</v>
-      </c>
-      <c r="E168" t="s">
-        <v>360</v>
       </c>
     </row>
     <row r="169" spans="2:5">
       <c r="B169" t="s">
+        <v>359</v>
+      </c>
+      <c r="C169" t="s">
+        <v>360</v>
+      </c>
+      <c r="D169" t="s">
         <v>361</v>
       </c>
-      <c r="C169" t="s">
+      <c r="E169" t="s">
         <v>362</v>
       </c>
-      <c r="D169" t="s">
+    </row>
+    <row r="170" spans="2:5">
+      <c r="B170" t="s">
         <v>363</v>
       </c>
-      <c r="E169" t="s">
+      <c r="C170" t="s">
         <v>364</v>
       </c>
-    </row>
-    <row r="170" s="3" customFormat="1" spans="1:1">
-      <c r="A170" s="3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="171" s="3" customFormat="1" spans="1:5">
+      <c r="D170" t="s">
+        <v>365</v>
+      </c>
+      <c r="E170" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="171" s="3" customFormat="1" spans="1:1">
       <c r="A171" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B171" s="10" t="s">
-        <v>365</v>
-      </c>
-      <c r="C171" s="10"/>
-      <c r="D171" s="10"/>
-      <c r="E171" s="10"/>
-    </row>
-    <row r="172" spans="2:5">
-      <c r="B172" t="s">
-        <v>366</v>
-      </c>
-      <c r="C172" t="s">
+    </row>
+    <row r="172" s="3" customFormat="1" spans="1:5">
+      <c r="A172" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B172" s="10" t="s">
         <v>367</v>
       </c>
-      <c r="D172" t="s">
+      <c r="C172" s="10"/>
+      <c r="D172" s="10"/>
+      <c r="E172" s="10"/>
+    </row>
+    <row r="173" spans="2:5">
+      <c r="B173" t="s">
         <v>368</v>
       </c>
-      <c r="E172" t="s">
-        <v>367</v>
+      <c r="C173" t="s">
+        <v>369</v>
+      </c>
+      <c r="D173" t="s">
+        <v>370</v>
+      </c>
+      <c r="E173" t="s">
+        <v>369</v>
       </c>
     </row>
   </sheetData>
@@ -4623,9 +4643,9 @@
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="D5:E5"/>
-    <mergeCell ref="B162:E162"/>
-    <mergeCell ref="B166:E166"/>
-    <mergeCell ref="B171:E171"/>
+    <mergeCell ref="B163:E163"/>
+    <mergeCell ref="B167:E167"/>
+    <mergeCell ref="B172:E172"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>